<commit_message>
Separacion de archivos, verificar IP consultas.
</commit_message>
<xml_diff>
--- a/Reporte_Puertos.xlsx
+++ b/Reporte_Puertos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dicofra1-my.sharepoint.com/personal/angel_liceaga_dicofra_com_mx/Documents/Documentos/Progra/CSOC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_FA4F01671C5074413C7F6329EE463D6DB9B8A617" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B5B6534-27B6-4C82-9142-13C7AAFB7B5C}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_C7DF617A68B0F25E2E2D7F2DF6BB3D6E9DB459E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAE6051B-E30E-4A86-9CF6-E49115A5169E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,12 +16,25 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Reporte Network" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="76">
   <si>
     <t>Time</t>
   </si>
@@ -56,31 +69,61 @@
     <t>IP Source</t>
   </si>
   <si>
-    <t>May 12, 2024 11:48:51</t>
-  </si>
-  <si>
-    <t>May 12, 2024 11:43:51</t>
-  </si>
-  <si>
-    <t>May 12, 2024 11:38:49</t>
-  </si>
-  <si>
-    <t>May 12, 2024 11:33:48</t>
-  </si>
-  <si>
-    <t>May 12, 2024 11:28:46</t>
-  </si>
-  <si>
-    <t>May 12, 2024 11:23:45</t>
-  </si>
-  <si>
-    <t>May 12, 2024 11:18:44</t>
-  </si>
-  <si>
-    <t>May 12, 2024 11:13:43</t>
-  </si>
-  <si>
-    <t>May 12, 2024 11:08:41</t>
+    <t>May 25, 2024 14:28:33</t>
+  </si>
+  <si>
+    <t>May 25, 2024 13:50:27</t>
+  </si>
+  <si>
+    <t>May 25, 2024 13:20:18</t>
+  </si>
+  <si>
+    <t>May 25, 2024 13:11:05</t>
+  </si>
+  <si>
+    <t>May 25, 2024 12:33:19</t>
+  </si>
+  <si>
+    <t>May 25, 2024 11:59:56</t>
+  </si>
+  <si>
+    <t>May 25, 2024 11:23:36</t>
+  </si>
+  <si>
+    <t>May 25, 2024 11:16:44</t>
+  </si>
+  <si>
+    <t>May 25, 2024 11:06:52</t>
+  </si>
+  <si>
+    <t>May 25, 2024 10:50:53</t>
+  </si>
+  <si>
+    <t>May 25, 2024 10:14:05</t>
+  </si>
+  <si>
+    <t>May 25, 2024 09:46:34</t>
+  </si>
+  <si>
+    <t>May 25, 2024 09:37:35</t>
+  </si>
+  <si>
+    <t>May 25, 2024 09:09:09</t>
+  </si>
+  <si>
+    <t>May 25, 2024 09:04:28</t>
+  </si>
+  <si>
+    <t>May 25, 2024 08:23:25</t>
+  </si>
+  <si>
+    <t>May 25, 2024 07:45:36</t>
+  </si>
+  <si>
+    <t>May 25, 2024 07:16:52</t>
+  </si>
+  <si>
+    <t>May 25, 2024 07:09:53</t>
   </si>
   <si>
     <t>Warning</t>
@@ -92,130 +135,221 @@
     <t>Agent</t>
   </si>
   <si>
-    <t>gsntpserver.gseguros.com.mx (10.1.1.234)</t>
+    <t>GDLNVR7</t>
+  </si>
+  <si>
+    <t>PVR-WIN-NAS</t>
   </si>
   <si>
     <t>System</t>
   </si>
   <si>
-    <t>hb34s-488</t>
-  </si>
-  <si>
-    <t>hb30s-488</t>
-  </si>
-  <si>
-    <t>hb32s-488</t>
-  </si>
-  <si>
-    <t>hb26s-488</t>
-  </si>
-  <si>
-    <t>hb28s-488</t>
-  </si>
-  <si>
-    <t>hb25s-488</t>
-  </si>
-  <si>
-    <t>hb31s-488</t>
-  </si>
-  <si>
-    <t>hb37s-488</t>
-  </si>
-  <si>
-    <t>hb35s-488</t>
-  </si>
-  <si>
-    <t>The Agent/Appliance detected an attempt to scan a computer or a network. Check the Agent/Appliance Events to see the details of the scan.
-Agent/Appliance Event(s):
-Time: May 12, 2024 11:48:48
-Level: Warning
-Event ID: 7001
-Event: Network or Port Scan
-Description: The computer at IP address 10.1.1.101 is performing a computer or network scan. It has scanned or attempted to scan a total of one computer.
-Traffic from IP 10.1.1.101 is not being automatically blocked.</t>
-  </si>
-  <si>
-    <t>The Agent/Appliance detected an attempt to scan a computer or a network. Check the Agent/Appliance Events to see the details of the scan.
-Agent/Appliance Event(s):
-Time: May 12, 2024 11:43:47
-Level: Warning
-Event ID: 7001
-Event: Network or Port Scan
-Description: The computer at IP address 10.1.1.101 is performing a computer or network scan. It has scanned or attempted to scan a total of one computer.
-Traffic from IP 10.1.1.101 is not being automatically blocked.</t>
-  </si>
-  <si>
-    <t>The Agent/Appliance detected an attempt to scan a computer or a network. Check the Agent/Appliance Events to see the details of the scan.
-Agent/Appliance Event(s):
-Time: May 12, 2024 11:38:46
-Level: Warning
-Event ID: 7001
-Event: Network or Port Scan
-Description: The computer at IP address 10.1.1.101 is performing a computer or network scan. It has scanned or attempted to scan a total of one computer.
-Traffic from IP 10.1.1.101 is not being automatically blocked.</t>
-  </si>
-  <si>
-    <t>The Agent/Appliance detected an attempt to scan a computer or a network. Check the Agent/Appliance Events to see the details of the scan.
-Agent/Appliance Event(s):
-Time: May 12, 2024 11:33:44
-Level: Warning
-Event ID: 7001
-Event: Network or Port Scan
-Description: The computer at IP address 10.1.1.101 is performing a computer or network scan. It has scanned or attempted to scan a total of one computer.
-Traffic from IP 10.1.1.101 is not being automatically blocked.</t>
-  </si>
-  <si>
-    <t>The Agent/Appliance detected an attempt to scan a computer or a network. Check the Agent/Appliance Events to see the details of the scan.
-Agent/Appliance Event(s):
-Time: May 12, 2024 11:28:43
-Level: Warning
-Event ID: 7001
-Event: Network or Port Scan
-Description: The computer at IP address 10.1.1.101 is performing a computer or network scan. It has scanned or attempted to scan a total of one computer.
-Traffic from IP 10.1.1.101 is not being automatically blocked.</t>
-  </si>
-  <si>
-    <t>The Agent/Appliance detected an attempt to scan a computer or a network. Check the Agent/Appliance Events to see the details of the scan.
-Agent/Appliance Event(s):
-Time: May 12, 2024 11:23:42
-Level: Warning
-Event ID: 7001
-Event: Network or Port Scan
-Description: The computer at IP address 10.1.1.101 is performing a computer or network scan. It has scanned or attempted to scan a total of one computer.
-Traffic from IP 10.1.1.101 is not being automatically blocked.</t>
-  </si>
-  <si>
-    <t>The Agent/Appliance detected an attempt to scan a computer or a network. Check the Agent/Appliance Events to see the details of the scan.
-Agent/Appliance Event(s):
-Time: May 12, 2024 11:18:40
-Level: Warning
-Event ID: 7001
-Event: Network or Port Scan
-Description: The computer at IP address 10.1.1.101 is performing a computer or network scan. It has scanned or attempted to scan a total of one computer.
-Traffic from IP 10.1.1.101 is not being automatically blocked.</t>
-  </si>
-  <si>
-    <t>The Agent/Appliance detected an attempt to scan a computer or a network. Check the Agent/Appliance Events to see the details of the scan.
-Agent/Appliance Event(s):
-Time: May 12, 2024 11:13:39
-Level: Warning
-Event ID: 7001
-Event: Network or Port Scan
-Description: The computer at IP address 10.1.1.101 is performing a computer or network scan. It has scanned or attempted to scan a total of one computer.
-Traffic from IP 10.1.1.101 is not being automatically blocked.</t>
-  </si>
-  <si>
-    <t>The Agent/Appliance detected an attempt to scan a computer or a network. Check the Agent/Appliance Events to see the details of the scan.
-Agent/Appliance Event(s):
-Time: May 12, 2024 11:08:38
-Level: Warning
-Event ID: 7001
-Event: Network or Port Scan
-Description: The computer at IP address 10.1.1.101 is performing a computer or network scan. It has scanned or attempted to scan a total of one computer.
-Traffic from IP 10.1.1.101 is not being automatically blocked.</t>
-  </si>
-  <si>
-    <t>10.1.1.101</t>
+    <t>10.255.130.184</t>
+  </si>
+  <si>
+    <t>The Agent/Appliance detected an attempt to scan a computer or a network. Check the Agent/Appliance Events to see the details of the scan.
+Agent/Appliance Event(s):
+Time: May 25, 2024 14:28:32
+Level: Warning
+Event ID: 7001
+Event: Network or Port Scan
+Description: The computer at IP address 10.223.200.13 is performing a computer or network scan. It has scanned or attempted to scan a total of one computer.
+Traffic from IP 10.223.200.13 is being automatically blocked for 1,800 seconds.</t>
+  </si>
+  <si>
+    <t>The Agent/Appliance detected an attempt to scan a computer or a network. Check the Agent/Appliance Events to see the details of the scan.
+Agent/Appliance Event(s):
+Time: May 25, 2024 13:50:25
+Level: Warning
+Event ID: 7001
+Event: Network or Port Scan
+Description: The computer at IP address 10.223.200.13 is performing a computer or network scan. It has scanned or attempted to scan a total of one computer.
+Traffic from IP 10.223.200.13 is being automatically blocked for 1,800 seconds.</t>
+  </si>
+  <si>
+    <t>The Agent/Appliance detected an attempt to scan a computer or a network. Check the Agent/Appliance Events to see the details of the scan.
+Agent/Appliance Event(s):
+Time: May 25, 2024 13:08:59
+Level: Warning
+Event ID: 7001
+Event: Network or Port Scan
+Description: The computer at IP address 10.219.200.11 is performing a computer or network scan. It has scanned or attempted to scan a total of 19 computers.
+Traffic from IP 10.219.200.11 is being automatically blocked for 1,800 seconds.</t>
+  </si>
+  <si>
+    <t>The Agent/Appliance detected an attempt to scan a computer or a network. Check the Agent/Appliance Events to see the details of the scan.
+Agent/Appliance Event(s):
+Time: May 25, 2024 13:11:04
+Level: Warning
+Event ID: 7001
+Event: Network or Port Scan
+Description: The computer at IP address 10.223.200.13 is performing a computer or network scan. It has scanned or attempted to scan a total of one computer.
+Traffic from IP 10.223.200.13 is being automatically blocked for 1,800 seconds.</t>
+  </si>
+  <si>
+    <t>The Agent/Appliance detected an attempt to scan a computer or a network. Check the Agent/Appliance Events to see the details of the scan.
+Agent/Appliance Event(s):
+Time: May 25, 2024 12:33:18
+Level: Warning
+Event ID: 7001
+Event: Network or Port Scan
+Description: The computer at IP address 10.223.200.13 is performing a computer or network scan. It has scanned or attempted to scan a total of one computer.
+Traffic from IP 10.223.200.13 is being automatically blocked for 1,800 seconds.</t>
+  </si>
+  <si>
+    <t>The Agent/Appliance detected an attempt to scan a computer or a network. Check the Agent/Appliance Events to see the details of the scan.
+Agent/Appliance Event(s):
+Time: May 25, 2024 11:59:55
+Level: Warning
+Event ID: 7001
+Event: Network or Port Scan
+Description: The computer at IP address 10.223.200.13 is performing a computer or network scan. It has scanned or attempted to scan a total of one computer.
+Traffic from IP 10.223.200.13 is being automatically blocked for 1,800 seconds.</t>
+  </si>
+  <si>
+    <t>The Agent/Appliance detected an attempt to scan a computer or a network. Check the Agent/Appliance Events to see the details of the scan.
+Agent/Appliance Event(s):
+Time: May 25, 2024 11:23:34
+Level: Warning
+Event ID: 7001
+Event: Network or Port Scan
+Description: The computer at IP address 10.223.200.13 is performing a computer or network scan. It has scanned or attempted to scan a total of one computer.
+Traffic from IP 10.223.200.13 is being automatically blocked for 1,800 seconds.</t>
+  </si>
+  <si>
+    <t>The Agent/Appliance detected an attempt to scan a computer or a network. Check the Agent/Appliance Events to see the details of the scan.
+Agent/Appliance Event(s):
+Time: May 25, 2024 11:05:25
+Level: Warning
+Event ID: 7001
+Event: Network or Port Scan
+Description: The computer at IP address 10.219.200.11 is performing a computer or network scan. It has scanned or attempted to scan a total of 20 computers.
+Traffic from IP 10.219.200.11 is being automatically blocked for 1,800 seconds.</t>
+  </si>
+  <si>
+    <t>The Agent/Appliance detected an attempt to scan a computer or a network. Check the Agent/Appliance Events to see the details of the scan.
+Agent/Appliance Event(s):
+Time: May 25, 2024 10:55:33
+Level: Warning
+Event ID: 7001
+Event: Network or Port Scan
+Description: The computer at IP address 10.219.200.12 is performing a computer or network scan. It has scanned or attempted to scan a total of 16 computers.
+Traffic from IP 10.219.200.12 is being automatically blocked for 1,800 seconds.</t>
+  </si>
+  <si>
+    <t>The Agent/Appliance detected an attempt to scan a computer or a network. Check the Agent/Appliance Events to see the details of the scan.
+Agent/Appliance Event(s):
+Time: May 25, 2024 10:50:51
+Level: Warning
+Event ID: 7001
+Event: Network or Port Scan
+Description: The computer at IP address 10.223.200.13 is performing a computer or network scan. It has scanned or attempted to scan a total of one computer.
+Traffic from IP 10.223.200.13 is being automatically blocked for 1,800 seconds.</t>
+  </si>
+  <si>
+    <t>The Agent/Appliance detected an attempt to scan a computer or a network. Check the Agent/Appliance Events to see the details of the scan.
+Agent/Appliance Event(s):
+Time: May 25, 2024 10:14:04
+Level: Warning
+Event ID: 7001
+Event: Network or Port Scan
+Description: The computer at IP address 10.223.200.13 is performing a computer or network scan. It has scanned or attempted to scan a total of one computer.
+Traffic from IP 10.223.200.13 is being automatically blocked for 1,800 seconds.</t>
+  </si>
+  <si>
+    <t>The Agent/Appliance detected an attempt to scan a computer or a network. Check the Agent/Appliance Events to see the details of the scan.
+Agent/Appliance Event(s):
+Time: May 25, 2024 09:35:15
+Level: Warning
+Event ID: 7001
+Event: Network or Port Scan
+Description: The computer at IP address 10.219.200.11 is performing a computer or network scan. It has scanned or attempted to scan a total of 24 computers.
+Traffic from IP 10.219.200.11 is being automatically blocked for 1,800 seconds.</t>
+  </si>
+  <si>
+    <t>The Agent/Appliance detected an attempt to scan a computer or a network. Check the Agent/Appliance Events to see the details of the scan.
+Agent/Appliance Event(s):
+Time: May 25, 2024 09:37:34
+Level: Warning
+Event ID: 7001
+Event: Network or Port Scan
+Description: The computer at IP address 10.223.200.13 is performing a computer or network scan. It has scanned or attempted to scan a total of one computer.
+Traffic from IP 10.223.200.13 is being automatically blocked for 1,800 seconds.</t>
+  </si>
+  <si>
+    <t>The Agent/Appliance detected an attempt to scan a computer or a network. Check the Agent/Appliance Events to see the details of the scan.
+Agent/Appliance Event(s):
+Time: May 25, 2024 09:09:08
+Level: Warning
+Event ID: 7001
+Event: Network or Port Scan
+Description: The computer at IP address 199.232.194.2 is performing a computer or network scan. It has scanned or attempted to scan a total of one computer.
+Traffic from IP 199.232.194.2 is being automatically blocked for 1,800 seconds.</t>
+  </si>
+  <si>
+    <t>The Agent/Appliance detected an attempt to scan a computer or a network. Check the Agent/Appliance Events to see the details of the scan.
+Agent/Appliance Event(s):
+Time: May 25, 2024 09:04:27
+Level: Warning
+Event ID: 7001
+Event: Network or Port Scan
+Description: The computer at IP address 10.223.200.13 is performing a computer or network scan. It has scanned or attempted to scan a total of one computer.
+Traffic from IP 10.223.200.13 is being automatically blocked for 1,800 seconds.</t>
+  </si>
+  <si>
+    <t>The Agent/Appliance detected an attempt to scan a computer or a network. Check the Agent/Appliance Events to see the details of the scan.
+Agent/Appliance Event(s):
+Time: May 25, 2024 08:23:24
+Level: Warning
+Event ID: 7001
+Event: Network or Port Scan
+Description: The computer at IP address 10.223.200.13 is performing a computer or network scan. It has scanned or attempted to scan a total of one computer.
+Traffic from IP 10.223.200.13 is being automatically blocked for 1,800 seconds.</t>
+  </si>
+  <si>
+    <t>The Agent/Appliance detected an attempt to scan a computer or a network. Check the Agent/Appliance Events to see the details of the scan.
+Agent/Appliance Event(s):
+Time: May 25, 2024 07:45:35
+Level: Warning
+Event ID: 7001
+Event: Network or Port Scan
+Description: The computer at IP address 10.223.200.13 is performing a computer or network scan. It has scanned or attempted to scan a total of one computer.
+Traffic from IP 10.223.200.13 is being automatically blocked for 1,800 seconds.</t>
+  </si>
+  <si>
+    <t>The Agent/Appliance detected an attempt to scan a computer or a network. Check the Agent/Appliance Events to see the details of the scan.
+Agent/Appliance Event(s):
+Time: May 25, 2024 07:16:51
+Level: Warning
+Event ID: 7001
+Event: Network or Port Scan
+Description: The computer at IP address 10.223.127.11 is performing a computer or network scan. It has scanned or attempted to scan a total of one computer.
+Traffic from IP 10.223.127.11 is being automatically blocked for 1,800 seconds.</t>
+  </si>
+  <si>
+    <t>The Agent/Appliance detected an attempt to scan a computer or a network. Check the Agent/Appliance Events to see the details of the scan.
+Agent/Appliance Event(s):
+Time: May 25, 2024 07:09:52
+Level: Warning
+Event ID: 7001
+Event: Network or Port Scan
+Description: The computer at IP address 10.223.200.13 is performing a computer or network scan. It has scanned or attempted to scan a total of one computer.
+Traffic from IP 10.223.200.13 is being automatically blocked for 1,800 seconds.</t>
+  </si>
+  <si>
+    <t>10.223.200.13</t>
+  </si>
+  <si>
+    <t>10.219.200.11</t>
+  </si>
+  <si>
+    <t>10.219.200.12</t>
+  </si>
+  <si>
+    <t>199.232.194.2</t>
+  </si>
+  <si>
+    <t>10.223.127.11</t>
   </si>
   <si>
     <t>Source IP</t>
@@ -246,6 +380,21 @@
   </si>
   <si>
     <t>Eventos:</t>
+  </si>
+  <si>
+    <t>10[.]223[.]127[.]11</t>
+  </si>
+  <si>
+    <t>10[.]223[.]200[.]13</t>
+  </si>
+  <si>
+    <t>199[.]232[.]194[.]2</t>
+  </si>
+  <si>
+    <t>10[.]219[.]200[.]11</t>
+  </si>
+  <si>
+    <t>10[.]219[.]200[.]12</t>
   </si>
 </sst>
 </file>
@@ -318,12 +467,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -632,7 +784,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -678,31 +830,31 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C2">
         <v>851</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="I2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="J2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="K2" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -710,31 +862,31 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C3">
         <v>851</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="J3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="K3" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -742,31 +894,31 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C4">
         <v>851</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="I4" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="J4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="K4" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -774,31 +926,31 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C5">
         <v>851</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="H5" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="I5" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="J5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K5" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -806,31 +958,31 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>851</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="G6" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="H6" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="I6" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="J6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K6" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -838,31 +990,31 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C7">
         <v>851</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="G7" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="H7" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="I7" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="K7" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -870,31 +1022,31 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C8">
         <v>851</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F8" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="G8" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="H8" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="I8" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J8" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K8" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -902,31 +1054,31 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C9">
         <v>851</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F9" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="G9" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="H9" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="I9" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="J9" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="K9" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -934,31 +1086,351 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10">
+        <v>851</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="C10">
-        <v>851</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <v>851</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" t="s">
+        <v>36</v>
+      </c>
+      <c r="J11" t="s">
+        <v>46</v>
+      </c>
+      <c r="K11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>21</v>
       </c>
-      <c r="F10" t="s">
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12">
+        <v>851</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" t="s">
+        <v>47</v>
+      </c>
+      <c r="K12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="G10" t="s">
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13">
+        <v>851</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" t="s">
+        <v>48</v>
+      </c>
+      <c r="K13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>23</v>
       </c>
-      <c r="H10" t="s">
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14">
+        <v>851</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" t="s">
+        <v>36</v>
+      </c>
+      <c r="J14" t="s">
+        <v>49</v>
+      </c>
+      <c r="K14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>24</v>
       </c>
-      <c r="I10" t="s">
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <v>851</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" t="s">
         <v>33</v>
       </c>
-      <c r="J10" t="s">
-        <v>42</v>
-      </c>
-      <c r="K10" t="s">
-        <v>43</v>
+      <c r="H15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" t="s">
+        <v>36</v>
+      </c>
+      <c r="J15" t="s">
+        <v>50</v>
+      </c>
+      <c r="K15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16">
+        <v>851</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" t="s">
+        <v>36</v>
+      </c>
+      <c r="J16" t="s">
+        <v>51</v>
+      </c>
+      <c r="K16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17">
+        <v>851</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J17" t="s">
+        <v>52</v>
+      </c>
+      <c r="K17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18">
+        <v>851</v>
+      </c>
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" t="s">
+        <v>36</v>
+      </c>
+      <c r="J18" t="s">
+        <v>53</v>
+      </c>
+      <c r="K18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19">
+        <v>851</v>
+      </c>
+      <c r="D19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I19" t="s">
+        <v>36</v>
+      </c>
+      <c r="J19" t="s">
+        <v>54</v>
+      </c>
+      <c r="K19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20">
+        <v>851</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" t="s">
+        <v>36</v>
+      </c>
+      <c r="J20" t="s">
+        <v>55</v>
+      </c>
+      <c r="K20" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -968,20 +1440,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.7109375" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="3" max="3" width="42.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="44" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="47.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -995,80 +1469,154 @@
         <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>23</v>
+      <c r="A2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="E2" s="3">
-        <v>9</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>50</v>
+        <v>1</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>49</v>
-      </c>
+      <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="2">
-        <v>9</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="D3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="3">
+        <v>13</v>
+      </c>
+      <c r="G3" s="4"/>
       <c r="H3" s="3" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G4" s="3" t="s">
-        <v>52</v>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="3">
-        <v>9</v>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="3">
+        <v>3</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="2">
+        <v>19</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G8" s="4"/>
+      <c r="H8" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G10" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="3">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A3:D3"/>
+  <mergeCells count="7">
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="G4:G8"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="A7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>